<commit_message>
search function and website function
</commit_message>
<xml_diff>
--- a/sensor test 1.0 .xlsx
+++ b/sensor test 1.0 .xlsx
@@ -164,7 +164,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -217,7 +217,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,7 +575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21" customFormat="1" s="3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -589,7 +589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="28.5" customFormat="1" s="3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33" customFormat="1" s="3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -603,7 +603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="28.5" customFormat="1" s="3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33" customFormat="1" s="3">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -617,7 +617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21" customFormat="1" s="3">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
new version of website
</commit_message>
<xml_diff>
--- a/sensor test 1.0 .xlsx
+++ b/sensor test 1.0 .xlsx
@@ -115,6 +115,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="2"/>
@@ -122,12 +128,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -167,14 +167,11 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -493,10 +490,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="43.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="43.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" customFormat="1" s="1">
@@ -507,7 +504,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -587,133 +584,133 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="60" customFormat="1" s="1">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="60" customFormat="1" s="1">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="62.25" customFormat="1" s="1">
-      <c r="A11" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="60" customFormat="1" s="1">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="60" customFormat="1" s="1">
+      <c r="A12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="62.25" customFormat="1" s="1">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="A15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="51" customFormat="1" s="1">
-      <c r="A16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="62.25" customFormat="1" s="1">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -727,7 +724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -741,7 +738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -755,7 +752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -769,7 +766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -783,7 +780,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
@@ -797,7 +794,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -811,7 +808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -825,7 +822,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>